<commit_message>
computed the top 5 attributes with higher loadings on each pca
</commit_message>
<xml_diff>
--- a/selected_attributes.xlsx
+++ b/selected_attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mugisha/Desktop/clone/watershed_classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF35E58-C9EC-D340-8F50-B049396EFAD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A54D5AD-483A-C04C-B1EE-BAEEF770EF52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{7C214A40-3DC1-8B4B-99AA-6AD5E40DD3EE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20280" xr2:uid="{7C214A40-3DC1-8B4B-99AA-6AD5E40DD3EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -515,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{288497FF-E818-9B47-958C-408F5FB9383C}">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>